<commit_message>
added sensors and motors to coordination sheet
</commit_message>
<xml_diff>
--- a/documentations/2022 coordination sheet.xlsx
+++ b/documentations/2022 coordination sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minni\Documents\GitHub\2022_prod_robot\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA30434-004C-4A9D-9706-F3A08D9F4C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F01730-8EAB-435A-B71E-ADCD6BC58575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3526,8 +3526,8 @@
   </sheetPr>
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
worked on sliding climb command
</commit_message>
<xml_diff>
--- a/documentations/2022 coordination sheet.xlsx
+++ b/documentations/2022 coordination sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minni\Documents\GitHub\2022_prod_robot\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC027E07-9E2A-4052-B502-E42530600AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28211AC-EC78-4DFD-A082-38903C19C3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -901,12 +901,6 @@
     <t>PDP 6</t>
   </si>
   <si>
-    <t>Magnet belt left</t>
-  </si>
-  <si>
-    <t>Magnet belt right</t>
-  </si>
-  <si>
     <t>ID-9</t>
   </si>
   <si>
@@ -966,6 +960,12 @@
   </si>
   <si>
     <t>SPI</t>
+  </si>
+  <si>
+    <t>Climb hook left</t>
+  </si>
+  <si>
+    <t>Climb hook right</t>
   </si>
 </sst>
 </file>
@@ -3526,8 +3526,8 @@
   </sheetPr>
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3573,7 +3573,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>4</v>
@@ -3907,7 +3907,7 @@
     </row>
     <row r="13" spans="1:13" ht="24">
       <c r="A13" s="3" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>108</v>
@@ -3944,7 +3944,7 @@
     </row>
     <row r="14" spans="1:13" ht="24">
       <c r="A14" s="31" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="B14" s="101" t="s">
         <v>108</v>
@@ -3959,13 +3959,13 @@
         <v>108</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G14" s="32" t="s">
         <v>166</v>
       </c>
       <c r="H14" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I14" s="32">
         <v>40</v>
@@ -3996,13 +3996,13 @@
         <v>108</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G15" s="32" t="s">
         <v>134</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I15" s="103">
         <v>40</v>
@@ -4018,24 +4018,24 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="C16" s="71" t="s">
         <v>202</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="C16" s="71" t="s">
-        <v>204</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="32"/>
       <c r="F16" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H16" s="32" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I16" s="103"/>
       <c r="J16" s="32" t="s">
@@ -4186,10 +4186,10 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C23" s="73" t="s">
         <v>68</v>
@@ -4209,7 +4209,7 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>67</v>
@@ -4364,16 +4364,16 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>209</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>211</v>
       </c>
       <c r="C31" s="73" t="s">
         <v>132</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E31" s="24">
         <v>11</v>

</xml_diff>

<commit_message>
added vertical climb subsystem and commands
</commit_message>
<xml_diff>
--- a/documentations/2022 coordination sheet.xlsx
+++ b/documentations/2022 coordination sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minni\Documents\GitHub\2022_prod_robot\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28211AC-EC78-4DFD-A082-38903C19C3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5183AA7-B0A1-4F1B-9A8E-4E518AB1AC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -649,12 +649,6 @@
     <t>Inverted (yes/no)/sensor phase (true/false)</t>
   </si>
   <si>
-    <t>climb motor left</t>
-  </si>
-  <si>
-    <t>climb motor right</t>
-  </si>
-  <si>
     <t>Bag motor</t>
   </si>
   <si>
@@ -966,6 +960,12 @@
   </si>
   <si>
     <t>Climb hook right</t>
+  </si>
+  <si>
+    <t>vertical climb motor left</t>
+  </si>
+  <si>
+    <t>vertical climb motor right</t>
   </si>
 </sst>
 </file>
@@ -3526,8 +3526,8 @@
   </sheetPr>
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3573,7 +3573,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>4</v>
@@ -3635,7 +3635,7 @@
         <v>10</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>28</v>
@@ -3667,7 +3667,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I6" s="102">
         <v>40</v>
@@ -3676,7 +3676,7 @@
         <v>10</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>28</v>
@@ -3717,7 +3717,7 @@
         <v>10</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>64</v>
@@ -3747,7 +3747,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I8" s="102">
         <v>40</v>
@@ -3756,7 +3756,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>64</v>
@@ -3765,16 +3765,16 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C9" s="71" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>24</v>
@@ -3786,26 +3786,26 @@
         <v>80</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I9" s="10">
         <v>30</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C10" s="71" t="s">
         <v>25</v>
@@ -3817,34 +3817,34 @@
         <v>24</v>
       </c>
       <c r="F10" s="39" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I10" s="10">
         <v>30</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L10" s="10"/>
       <c r="M10" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C11" s="71" t="s">
         <v>25</v>
@@ -3854,13 +3854,13 @@
         <v>24</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I11" s="10">
         <v>30</v>
@@ -3869,33 +3869,33 @@
         <v>10</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C12" s="71" t="s">
         <v>189</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="C12" s="71" t="s">
-        <v>191</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>194</v>
       </c>
       <c r="I12" s="10">
         <v>20</v>
@@ -3907,7 +3907,7 @@
     </row>
     <row r="13" spans="1:13" ht="24">
       <c r="A13" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>108</v>
@@ -3922,10 +3922,10 @@
         <v>108</v>
       </c>
       <c r="F13" s="39" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>81</v>
@@ -3937,14 +3937,14 @@
         <v>10</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L13" s="10"/>
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" ht="24">
       <c r="A14" s="31" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B14" s="101" t="s">
         <v>108</v>
@@ -3959,13 +3959,13 @@
         <v>108</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H14" s="32" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I14" s="32">
         <v>40</v>
@@ -3974,14 +3974,14 @@
         <v>10</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L14" s="10"/>
       <c r="M14" s="33"/>
     </row>
     <row r="15" spans="1:13" ht="24">
       <c r="A15" s="31" t="s">
-        <v>111</v>
+        <v>211</v>
       </c>
       <c r="B15" s="32" t="s">
         <v>108</v>
@@ -3996,13 +3996,13 @@
         <v>108</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I15" s="103">
         <v>40</v>
@@ -4011,35 +4011,35 @@
         <v>10</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L15" s="10"/>
       <c r="M15" s="33"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="C16" s="71" t="s">
         <v>200</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>201</v>
-      </c>
-      <c r="C16" s="71" t="s">
-        <v>202</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="32"/>
       <c r="F16" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H16" s="32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I16" s="103"/>
       <c r="J16" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K16" s="12"/>
       <c r="L16" s="10"/>
@@ -4047,7 +4047,7 @@
     </row>
     <row r="17" spans="1:13" ht="24.6" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>112</v>
+        <v>212</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>108</v>
@@ -4062,13 +4062,13 @@
         <v>108</v>
       </c>
       <c r="F17" s="39" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I17" s="104">
         <v>40</v>
@@ -4077,7 +4077,7 @@
         <v>10</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="29"/>
@@ -4186,10 +4186,10 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C23" s="73" t="s">
         <v>68</v>
@@ -4209,7 +4209,7 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>67</v>
@@ -4234,16 +4234,16 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="73" t="s">
         <v>126</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="D25" s="10" t="s">
         <v>127</v>
-      </c>
-      <c r="C25" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>129</v>
       </c>
       <c r="E25" s="24">
         <v>4</v>
@@ -4259,16 +4259,16 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="83" t="s">
+        <v>128</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="73" t="s">
         <v>130</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="D26" s="10" t="s">
         <v>131</v>
-      </c>
-      <c r="C26" s="73" t="s">
-        <v>132</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="E26" s="24">
         <v>5</v>
@@ -4284,16 +4284,16 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>170</v>
-      </c>
       <c r="C27" s="73" t="s">
+        <v>167</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>169</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>171</v>
       </c>
       <c r="E27" s="24">
         <v>6</v>
@@ -4309,16 +4309,16 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B28" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C28" s="73" t="s">
+        <v>167</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>170</v>
-      </c>
-      <c r="C28" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>172</v>
       </c>
       <c r="E28" s="36">
         <v>7</v>
@@ -4364,16 +4364,16 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>209</v>
-      </c>
       <c r="C31" s="73" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E31" s="24">
         <v>11</v>
@@ -4389,16 +4389,16 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C32" s="73" t="s">
+        <v>176</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>178</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>180</v>
       </c>
       <c r="E32" s="24">
         <v>8</v>
@@ -4414,16 +4414,16 @@
     </row>
     <row r="33" spans="1:13" ht="15" thickBot="1">
       <c r="A33" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C33" s="74" t="s">
+        <v>177</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>179</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>181</v>
       </c>
       <c r="E33" s="23">
         <v>9</v>
@@ -4937,7 +4937,7 @@
         <v>70</v>
       </c>
       <c r="B64" s="43" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C64" s="79">
         <v>2</v>
@@ -4957,7 +4957,7 @@
         <v>70</v>
       </c>
       <c r="B65" s="43" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C65" s="79">
         <v>3</v>
@@ -4977,7 +4977,7 @@
         <v>70</v>
       </c>
       <c r="B66" s="43" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C66" s="80">
         <v>4</v>
@@ -4997,7 +4997,7 @@
         <v>70</v>
       </c>
       <c r="B67" s="43" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C67" s="80">
         <v>5</v>
@@ -5017,7 +5017,7 @@
         <v>70</v>
       </c>
       <c r="B68" s="43" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C68" s="80">
         <v>6</v>
@@ -5037,7 +5037,7 @@
         <v>70</v>
       </c>
       <c r="B69" s="43" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C69" s="80">
         <v>8</v>
@@ -5089,7 +5089,7 @@
         <v>79</v>
       </c>
       <c r="B72" s="39" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C72" s="80">
         <v>1</v>
@@ -5107,7 +5107,7 @@
         <v>79</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C73" s="71">
         <v>2</v>
@@ -5136,7 +5136,7 @@
       <c r="K74" s="61"/>
       <c r="L74"/>
       <c r="M74" s="92" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="N74" s="93"/>
       <c r="O74" s="94"/>
@@ -5146,7 +5146,7 @@
         <v>79</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C75" s="71">
         <v>4</v>
@@ -5159,7 +5159,7 @@
       <c r="K75" s="61"/>
       <c r="L75"/>
       <c r="M75" s="95" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N75" s="39"/>
       <c r="O75" s="96"/>
@@ -5169,7 +5169,7 @@
         <v>79</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C76" s="71">
         <v>5</v>
@@ -5182,7 +5182,7 @@
       <c r="K76" s="61"/>
       <c r="L76"/>
       <c r="M76" s="95" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N76" s="39"/>
       <c r="O76" s="96"/>
@@ -5192,7 +5192,7 @@
         <v>79</v>
       </c>
       <c r="B77" s="91" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C77" s="71">
         <v>6</v>
@@ -5205,7 +5205,7 @@
       <c r="K77" s="61"/>
       <c r="L77"/>
       <c r="M77" s="95" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="N77" s="39"/>
       <c r="O77" s="96"/>
@@ -5215,7 +5215,7 @@
         <v>79</v>
       </c>
       <c r="B78" s="91" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C78" s="71">
         <v>7</v>
@@ -5228,7 +5228,7 @@
       <c r="K78" s="61"/>
       <c r="L78"/>
       <c r="M78" s="95" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="N78" s="10"/>
       <c r="O78" s="96"/>
@@ -5238,7 +5238,7 @@
         <v>79</v>
       </c>
       <c r="B79" s="91" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C79" s="71">
         <v>8</v>
@@ -5251,7 +5251,7 @@
       <c r="K79" s="61"/>
       <c r="L79"/>
       <c r="M79" s="95" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="N79" s="10"/>
       <c r="O79" s="96"/>
@@ -5261,7 +5261,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="91" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C80" s="71">
         <v>9</v>
@@ -5274,7 +5274,7 @@
       <c r="K80" s="61"/>
       <c r="L80"/>
       <c r="M80" s="95" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="N80" s="10"/>
       <c r="O80" s="96"/>
@@ -5284,7 +5284,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="91" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C81" s="71">
         <v>10</v>
@@ -5297,7 +5297,7 @@
       <c r="K81" s="61"/>
       <c r="L81"/>
       <c r="M81" s="95" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="N81" s="52"/>
       <c r="O81" s="96"/>
@@ -5307,7 +5307,7 @@
         <v>79</v>
       </c>
       <c r="B82" s="91" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C82" s="71">
         <v>1</v>
@@ -5320,7 +5320,7 @@
       <c r="K82" s="61"/>
       <c r="L82"/>
       <c r="M82" s="95" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="N82" s="39"/>
       <c r="O82" s="96"/>
@@ -5330,7 +5330,7 @@
         <v>79</v>
       </c>
       <c r="B83" s="91" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C83" s="71">
         <v>3</v>
@@ -5343,7 +5343,7 @@
       <c r="K83" s="61"/>
       <c r="L83"/>
       <c r="M83" s="95" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="N83" s="39"/>
       <c r="O83" s="96"/>
@@ -5360,7 +5360,7 @@
       <c r="K84" s="61"/>
       <c r="L84"/>
       <c r="M84" s="95" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="N84" s="65"/>
       <c r="O84" s="96"/>

</xml_diff>

<commit_message>
added stuff to autonomous
</commit_message>
<xml_diff>
--- a/documentations/2022 coordination sheet.xlsx
+++ b/documentations/2022 coordination sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minni\Documents\GitHub\2022_prod_robot\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5183AA7-B0A1-4F1B-9A8E-4E518AB1AC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0D370A-2E4B-420C-B76E-8B83AFA2C002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -655,9 +655,6 @@
     <t>mini CIM</t>
   </si>
   <si>
-    <t>Pigeon (Vinnie)</t>
-  </si>
-  <si>
     <t>ID-7</t>
   </si>
   <si>
@@ -967,12 +964,15 @@
   <si>
     <t>vertical climb motor right</t>
   </si>
+  <si>
+    <t>pigeon (vinnie)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1111,6 +1111,22 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1624,7 +1640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1935,6 +1951,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3527,7 +3564,7 @@
   <dimension ref="A1:O107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3573,7 +3610,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>4</v>
@@ -3623,10 +3660,10 @@
         <v>61</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>31</v>
+        <v>180</v>
       </c>
       <c r="I5" s="102">
         <v>40</v>
@@ -3635,7 +3672,7 @@
         <v>10</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>28</v>
@@ -3664,10 +3701,10 @@
         <v>63</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>180</v>
+        <v>82</v>
       </c>
       <c r="I6" s="102">
         <v>40</v>
@@ -3676,7 +3713,7 @@
         <v>10</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>28</v>
@@ -3705,10 +3742,10 @@
         <v>65</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>82</v>
+        <v>179</v>
       </c>
       <c r="I7" s="102">
         <v>40</v>
@@ -3717,7 +3754,7 @@
         <v>10</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>64</v>
@@ -3744,10 +3781,10 @@
         <v>66</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>181</v>
+        <v>31</v>
       </c>
       <c r="I8" s="102">
         <v>40</v>
@@ -3756,7 +3793,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>64</v>
@@ -3765,7 +3802,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>111</v>
@@ -3773,36 +3810,34 @@
       <c r="C9" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>113</v>
-      </c>
+      <c r="D9" s="17"/>
       <c r="E9" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="39" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>80</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I9" s="10">
         <v>30</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>111</v>
@@ -3817,31 +3852,31 @@
         <v>24</v>
       </c>
       <c r="F10" s="39" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I10" s="10">
         <v>30</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L10" s="10"/>
       <c r="M10" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>112</v>
@@ -3849,18 +3884,20 @@
       <c r="C11" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="17"/>
+      <c r="D11" s="17" t="s">
+        <v>212</v>
+      </c>
       <c r="E11" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I11" s="10">
         <v>30</v>
@@ -3869,45 +3906,45 @@
         <v>10</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:13" s="113" customFormat="1">
+      <c r="A12" s="107" t="s">
+        <v>186</v>
+      </c>
+      <c r="B12" s="108" t="s">
         <v>187</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="C12" s="109" t="s">
         <v>188</v>
       </c>
-      <c r="C12" s="71" t="s">
+      <c r="D12" s="110"/>
+      <c r="E12" s="111" t="s">
         <v>189</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="111" t="s">
         <v>190</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="111" t="s">
+        <v>161</v>
+      </c>
+      <c r="H12" s="111" t="s">
         <v>191</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="I12" s="10">
+      <c r="I12" s="111">
         <v>20</v>
       </c>
-      <c r="J12" s="10"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="4"/>
+      <c r="J12" s="111"/>
+      <c r="K12" s="108"/>
+      <c r="L12" s="111"/>
+      <c r="M12" s="112"/>
     </row>
     <row r="13" spans="1:13" ht="24">
       <c r="A13" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>108</v>
@@ -3922,10 +3959,10 @@
         <v>108</v>
       </c>
       <c r="F13" s="39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>81</v>
@@ -3937,14 +3974,14 @@
         <v>10</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L13" s="10"/>
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" ht="24">
       <c r="A14" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B14" s="101" t="s">
         <v>108</v>
@@ -3959,13 +3996,13 @@
         <v>108</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H14" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I14" s="32">
         <v>40</v>
@@ -3974,14 +4011,14 @@
         <v>10</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L14" s="10"/>
       <c r="M14" s="33"/>
     </row>
     <row r="15" spans="1:13" ht="24">
       <c r="A15" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B15" s="32" t="s">
         <v>108</v>
@@ -3996,13 +4033,13 @@
         <v>108</v>
       </c>
       <c r="F15" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="H15" s="32" t="s">
         <v>194</v>
-      </c>
-      <c r="G15" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="H15" s="32" t="s">
-        <v>195</v>
       </c>
       <c r="I15" s="103">
         <v>40</v>
@@ -4011,35 +4048,35 @@
         <v>10</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L15" s="10"/>
       <c r="M15" s="33"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="C16" s="71" t="s">
         <v>199</v>
-      </c>
-      <c r="C16" s="71" t="s">
-        <v>200</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="32"/>
       <c r="F16" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="G16" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="G16" s="32" t="s">
-        <v>202</v>
-      </c>
       <c r="H16" s="32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I16" s="103"/>
       <c r="J16" s="32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K16" s="12"/>
       <c r="L16" s="10"/>
@@ -4047,7 +4084,7 @@
     </row>
     <row r="17" spans="1:13" ht="24.6" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>108</v>
@@ -4062,13 +4099,13 @@
         <v>108</v>
       </c>
       <c r="F17" s="39" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I17" s="104">
         <v>40</v>
@@ -4077,7 +4114,7 @@
         <v>10</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="29"/>
@@ -4186,10 +4223,10 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>203</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>204</v>
       </c>
       <c r="C23" s="73" t="s">
         <v>68</v>
@@ -4209,7 +4246,7 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>67</v>
@@ -4234,16 +4271,16 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="83" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="C25" s="73" t="s">
         <v>125</v>
       </c>
-      <c r="C25" s="73" t="s">
+      <c r="D25" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>127</v>
       </c>
       <c r="E25" s="24">
         <v>4</v>
@@ -4259,16 +4296,16 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="83" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="C26" s="73" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="73" t="s">
+      <c r="D26" s="10" t="s">
         <v>130</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>131</v>
       </c>
       <c r="E26" s="24">
         <v>5</v>
@@ -4284,16 +4321,16 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="D27" s="10" t="s">
         <v>168</v>
-      </c>
-      <c r="C27" s="73" t="s">
-        <v>167</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>169</v>
       </c>
       <c r="E27" s="24">
         <v>6</v>
@@ -4309,16 +4346,16 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C28" s="73" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E28" s="36">
         <v>7</v>
@@ -4364,16 +4401,16 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B31" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C31" s="73" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>207</v>
-      </c>
-      <c r="C31" s="73" t="s">
-        <v>130</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>208</v>
       </c>
       <c r="E31" s="24">
         <v>11</v>
@@ -4389,16 +4426,16 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C32" s="73" t="s">
         <v>175</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C32" s="73" t="s">
-        <v>176</v>
-      </c>
       <c r="D32" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E32" s="24">
         <v>8</v>
@@ -4414,16 +4451,16 @@
     </row>
     <row r="33" spans="1:13" ht="15" thickBot="1">
       <c r="A33" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C33" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E33" s="23">
         <v>9</v>
@@ -4937,7 +4974,7 @@
         <v>70</v>
       </c>
       <c r="B64" s="43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C64" s="79">
         <v>2</v>
@@ -4957,7 +4994,7 @@
         <v>70</v>
       </c>
       <c r="B65" s="43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C65" s="79">
         <v>3</v>
@@ -4977,7 +5014,7 @@
         <v>70</v>
       </c>
       <c r="B66" s="43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C66" s="80">
         <v>4</v>
@@ -4997,7 +5034,7 @@
         <v>70</v>
       </c>
       <c r="B67" s="43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C67" s="80">
         <v>5</v>
@@ -5017,7 +5054,7 @@
         <v>70</v>
       </c>
       <c r="B68" s="43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C68" s="80">
         <v>6</v>
@@ -5037,7 +5074,7 @@
         <v>70</v>
       </c>
       <c r="B69" s="43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C69" s="80">
         <v>8</v>
@@ -5089,7 +5126,7 @@
         <v>79</v>
       </c>
       <c r="B72" s="39" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C72" s="80">
         <v>1</v>
@@ -5107,7 +5144,7 @@
         <v>79</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C73" s="71">
         <v>2</v>
@@ -5136,7 +5173,7 @@
       <c r="K74" s="61"/>
       <c r="L74"/>
       <c r="M74" s="92" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N74" s="93"/>
       <c r="O74" s="94"/>
@@ -5146,7 +5183,7 @@
         <v>79</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C75" s="71">
         <v>4</v>
@@ -5159,7 +5196,7 @@
       <c r="K75" s="61"/>
       <c r="L75"/>
       <c r="M75" s="95" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N75" s="39"/>
       <c r="O75" s="96"/>
@@ -5169,7 +5206,7 @@
         <v>79</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C76" s="71">
         <v>5</v>
@@ -5182,7 +5219,7 @@
       <c r="K76" s="61"/>
       <c r="L76"/>
       <c r="M76" s="95" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N76" s="39"/>
       <c r="O76" s="96"/>
@@ -5192,7 +5229,7 @@
         <v>79</v>
       </c>
       <c r="B77" s="91" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C77" s="71">
         <v>6</v>
@@ -5205,7 +5242,7 @@
       <c r="K77" s="61"/>
       <c r="L77"/>
       <c r="M77" s="95" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N77" s="39"/>
       <c r="O77" s="96"/>
@@ -5215,7 +5252,7 @@
         <v>79</v>
       </c>
       <c r="B78" s="91" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C78" s="71">
         <v>7</v>
@@ -5228,7 +5265,7 @@
       <c r="K78" s="61"/>
       <c r="L78"/>
       <c r="M78" s="95" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N78" s="10"/>
       <c r="O78" s="96"/>
@@ -5238,7 +5275,7 @@
         <v>79</v>
       </c>
       <c r="B79" s="91" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C79" s="71">
         <v>8</v>
@@ -5251,7 +5288,7 @@
       <c r="K79" s="61"/>
       <c r="L79"/>
       <c r="M79" s="95" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N79" s="10"/>
       <c r="O79" s="96"/>
@@ -5261,7 +5298,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="91" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C80" s="71">
         <v>9</v>
@@ -5274,7 +5311,7 @@
       <c r="K80" s="61"/>
       <c r="L80"/>
       <c r="M80" s="95" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N80" s="10"/>
       <c r="O80" s="96"/>
@@ -5284,7 +5321,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="91" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C81" s="71">
         <v>10</v>
@@ -5297,7 +5334,7 @@
       <c r="K81" s="61"/>
       <c r="L81"/>
       <c r="M81" s="95" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N81" s="52"/>
       <c r="O81" s="96"/>
@@ -5307,7 +5344,7 @@
         <v>79</v>
       </c>
       <c r="B82" s="91" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C82" s="71">
         <v>1</v>
@@ -5320,7 +5357,7 @@
       <c r="K82" s="61"/>
       <c r="L82"/>
       <c r="M82" s="95" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N82" s="39"/>
       <c r="O82" s="96"/>
@@ -5330,7 +5367,7 @@
         <v>79</v>
       </c>
       <c r="B83" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C83" s="71">
         <v>3</v>
@@ -5343,7 +5380,7 @@
       <c r="K83" s="61"/>
       <c r="L83"/>
       <c r="M83" s="95" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N83" s="39"/>
       <c r="O83" s="96"/>
@@ -5360,7 +5397,7 @@
       <c r="K84" s="61"/>
       <c r="L84"/>
       <c r="M84" s="95" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N84" s="65"/>
       <c r="O84" s="96"/>

</xml_diff>

<commit_message>
Added stuff to sliding climb hooks commands and subsystem
</commit_message>
<xml_diff>
--- a/documentations/2022 coordination sheet.xlsx
+++ b/documentations/2022 coordination sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minni\Documents\GitHub\2022_prod_robot\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0D370A-2E4B-420C-B76E-8B83AFA2C002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC6883C-8B6A-41F1-9B6A-F5D58F415137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -892,9 +892,6 @@
     <t>PDP 6</t>
   </si>
   <si>
-    <t>ID-9</t>
-  </si>
-  <si>
     <t>ID-10</t>
   </si>
   <si>
@@ -966,6 +963,9 @@
   </si>
   <si>
     <t>pigeon (vinnie)</t>
+  </si>
+  <si>
+    <t>ID-12</t>
   </si>
 </sst>
 </file>
@@ -1946,32 +1946,32 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3563,8 +3563,8 @@
   </sheetPr>
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3610,7 +3610,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>4</v>
@@ -3885,7 +3885,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>24</v>
@@ -3911,40 +3911,40 @@
       <c r="L11" s="10"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13" s="113" customFormat="1">
-      <c r="A12" s="107" t="s">
+    <row r="12" spans="1:13" s="111" customFormat="1">
+      <c r="A12" s="105" t="s">
         <v>186</v>
       </c>
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="106" t="s">
         <v>187</v>
       </c>
-      <c r="C12" s="109" t="s">
+      <c r="C12" s="107" t="s">
         <v>188</v>
       </c>
-      <c r="D12" s="110"/>
-      <c r="E12" s="111" t="s">
+      <c r="D12" s="108"/>
+      <c r="E12" s="109" t="s">
         <v>189</v>
       </c>
-      <c r="F12" s="111" t="s">
+      <c r="F12" s="109" t="s">
         <v>190</v>
       </c>
-      <c r="G12" s="111" t="s">
+      <c r="G12" s="109" t="s">
         <v>161</v>
       </c>
-      <c r="H12" s="111" t="s">
+      <c r="H12" s="109" t="s">
         <v>191</v>
       </c>
-      <c r="I12" s="111">
+      <c r="I12" s="109">
         <v>20</v>
       </c>
-      <c r="J12" s="111"/>
-      <c r="K12" s="108"/>
-      <c r="L12" s="111"/>
-      <c r="M12" s="112"/>
+      <c r="J12" s="109"/>
+      <c r="K12" s="106"/>
+      <c r="L12" s="109"/>
+      <c r="M12" s="110"/>
     </row>
     <row r="13" spans="1:13" ht="24">
       <c r="A13" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>108</v>
@@ -3959,13 +3959,13 @@
         <v>108</v>
       </c>
       <c r="F13" s="39" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>162</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>81</v>
+        <v>194</v>
       </c>
       <c r="I13" s="102">
         <v>40</v>
@@ -3981,7 +3981,7 @@
     </row>
     <row r="14" spans="1:13" ht="24">
       <c r="A14" s="31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B14" s="101" t="s">
         <v>108</v>
@@ -3996,13 +3996,13 @@
         <v>108</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="G14" s="32" t="s">
         <v>163</v>
       </c>
       <c r="H14" s="32" t="s">
-        <v>195</v>
+        <v>81</v>
       </c>
       <c r="I14" s="32">
         <v>40</v>
@@ -4018,7 +4018,7 @@
     </row>
     <row r="15" spans="1:13" ht="24">
       <c r="A15" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B15" s="32" t="s">
         <v>108</v>
@@ -4033,13 +4033,13 @@
         <v>108</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G15" s="32" t="s">
         <v>131</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I15" s="103">
         <v>40</v>
@@ -4055,24 +4055,24 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="B16" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="C16" s="71" t="s">
         <v>198</v>
-      </c>
-      <c r="C16" s="71" t="s">
-        <v>199</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="32"/>
       <c r="F16" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="G16" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="G16" s="32" t="s">
-        <v>201</v>
-      </c>
       <c r="H16" s="32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I16" s="103"/>
       <c r="J16" s="32" t="s">
@@ -4084,7 +4084,7 @@
     </row>
     <row r="17" spans="1:13" ht="24.6" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>108</v>
@@ -4099,7 +4099,7 @@
         <v>108</v>
       </c>
       <c r="F17" s="39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>122</v>
@@ -4223,10 +4223,10 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>202</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>203</v>
       </c>
       <c r="C23" s="73" t="s">
         <v>68</v>
@@ -4246,7 +4246,7 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>67</v>
@@ -4401,16 +4401,16 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C31" s="73" t="s">
         <v>129</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E31" s="24">
         <v>11</v>
@@ -4919,10 +4919,10 @@
       <c r="I61" s="45"/>
       <c r="J61" s="45"/>
       <c r="K61" s="60"/>
-      <c r="L61" s="105" t="s">
+      <c r="L61" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="M61" s="106" t="s">
+      <c r="M61" s="113" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4946,8 +4946,8 @@
       <c r="I62" s="39"/>
       <c r="J62" s="39"/>
       <c r="K62" s="61"/>
-      <c r="L62" s="105"/>
-      <c r="M62" s="106"/>
+      <c r="L62" s="112"/>
+      <c r="M62" s="113"/>
     </row>
     <row r="63" spans="1:14">
       <c r="A63" s="41" t="s">

</xml_diff>

<commit_message>
made sure both climbs work (they do!!!! tho there is a little motor whining)
</commit_message>
<xml_diff>
--- a/documentations/2022 coordination sheet.xlsx
+++ b/documentations/2022 coordination sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minni\Documents\GitHub\2022_prod_robot\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC6883C-8B6A-41F1-9B6A-F5D58F415137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73290C4-C60E-4D22-B224-2BB9BE6059FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3564,7 +3564,7 @@
   <dimension ref="A1:O107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
changed the PDP port for the right intake motor bc it was wrong
</commit_message>
<xml_diff>
--- a/documentations/2022 coordination sheet.xlsx
+++ b/documentations/2022 coordination sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minni\Documents\GitHub\2022_prod_robot\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73290C4-C60E-4D22-B224-2BB9BE6059FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEECA148-30E5-42B6-B978-BF5804F3612B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="212">
   <si>
     <t>Relay Function Chart</t>
   </si>
@@ -667,9 +667,6 @@
     <t>Bu</t>
   </si>
   <si>
-    <t>PDP 15</t>
-  </si>
-  <si>
     <t>PDP 3</t>
   </si>
   <si>
@@ -854,9 +851,6 @@
   </si>
   <si>
     <t>PDP 19</t>
-  </si>
-  <si>
-    <t>PDP 18</t>
   </si>
   <si>
     <t>Ball intake motor left</t>
@@ -966,6 +960,9 @@
   </si>
   <si>
     <t>ID-12</t>
+  </si>
+  <si>
+    <t>PDP 10</t>
   </si>
 </sst>
 </file>
@@ -3563,8 +3560,8 @@
   </sheetPr>
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3610,7 +3607,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>4</v>
@@ -3663,7 +3660,7 @@
         <v>8</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>180</v>
+        <v>119</v>
       </c>
       <c r="I5" s="102">
         <v>40</v>
@@ -3672,7 +3669,7 @@
         <v>10</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>28</v>
@@ -3713,7 +3710,7 @@
         <v>10</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>28</v>
@@ -3745,7 +3742,7 @@
         <v>7</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I7" s="102">
         <v>40</v>
@@ -3754,7 +3751,7 @@
         <v>10</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>64</v>
@@ -3793,7 +3790,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>64</v>
@@ -3802,7 +3799,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>111</v>
@@ -3821,23 +3818,23 @@
         <v>80</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I9" s="10">
         <v>30</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>111</v>
@@ -3852,31 +3849,31 @@
         <v>24</v>
       </c>
       <c r="F10" s="39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I10" s="10">
         <v>30</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L10" s="10"/>
       <c r="M10" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>112</v>
@@ -3885,7 +3882,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>24</v>
@@ -3897,7 +3894,7 @@
         <v>116</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>120</v>
+        <v>211</v>
       </c>
       <c r="I11" s="10">
         <v>30</v>
@@ -3906,33 +3903,33 @@
         <v>10</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:13" s="111" customFormat="1">
       <c r="A12" s="105" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="C12" s="107" t="s">
         <v>186</v>
-      </c>
-      <c r="B12" s="106" t="s">
-        <v>187</v>
-      </c>
-      <c r="C12" s="107" t="s">
-        <v>188</v>
       </c>
       <c r="D12" s="108"/>
       <c r="E12" s="109" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="109" t="s">
+        <v>188</v>
+      </c>
+      <c r="G12" s="109" t="s">
+        <v>160</v>
+      </c>
+      <c r="H12" s="109" t="s">
         <v>189</v>
-      </c>
-      <c r="F12" s="109" t="s">
-        <v>190</v>
-      </c>
-      <c r="G12" s="109" t="s">
-        <v>161</v>
-      </c>
-      <c r="H12" s="109" t="s">
-        <v>191</v>
       </c>
       <c r="I12" s="109">
         <v>20</v>
@@ -3944,7 +3941,7 @@
     </row>
     <row r="13" spans="1:13" ht="24">
       <c r="A13" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>108</v>
@@ -3962,10 +3959,10 @@
         <v>115</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I13" s="102">
         <v>40</v>
@@ -3974,14 +3971,14 @@
         <v>10</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L13" s="10"/>
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" ht="24">
       <c r="A14" s="31" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B14" s="101" t="s">
         <v>108</v>
@@ -3996,10 +3993,10 @@
         <v>108</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H14" s="32" t="s">
         <v>81</v>
@@ -4011,14 +4008,14 @@
         <v>10</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L14" s="10"/>
       <c r="M14" s="33"/>
     </row>
     <row r="15" spans="1:13" ht="24">
       <c r="A15" s="31" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B15" s="32" t="s">
         <v>108</v>
@@ -4033,13 +4030,13 @@
         <v>108</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I15" s="103">
         <v>40</v>
@@ -4048,35 +4045,35 @@
         <v>10</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L15" s="10"/>
       <c r="M15" s="33"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="C16" s="71" t="s">
         <v>196</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="C16" s="71" t="s">
-        <v>198</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="32"/>
       <c r="F16" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H16" s="32" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I16" s="103"/>
       <c r="J16" s="32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K16" s="12"/>
       <c r="L16" s="10"/>
@@ -4084,7 +4081,7 @@
     </row>
     <row r="17" spans="1:13" ht="24.6" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>108</v>
@@ -4102,10 +4099,10 @@
         <v>114</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I17" s="104">
         <v>40</v>
@@ -4114,7 +4111,7 @@
         <v>10</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="29"/>
@@ -4223,10 +4220,10 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C23" s="73" t="s">
         <v>68</v>
@@ -4246,7 +4243,7 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>67</v>
@@ -4271,16 +4268,16 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="83" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="C25" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="C25" s="73" t="s">
+      <c r="D25" s="10" t="s">
         <v>125</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>126</v>
       </c>
       <c r="E25" s="24">
         <v>4</v>
@@ -4296,16 +4293,16 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="83" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="C26" s="73" t="s">
         <v>128</v>
       </c>
-      <c r="C26" s="73" t="s">
+      <c r="D26" s="10" t="s">
         <v>129</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>130</v>
       </c>
       <c r="E26" s="24">
         <v>5</v>
@@ -4321,16 +4318,16 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C27" s="73" t="s">
         <v>165</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="D27" s="10" t="s">
         <v>167</v>
-      </c>
-      <c r="C27" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>168</v>
       </c>
       <c r="E27" s="24">
         <v>6</v>
@@ -4346,16 +4343,16 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C28" s="73" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E28" s="36">
         <v>7</v>
@@ -4401,16 +4398,16 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>205</v>
-      </c>
       <c r="C31" s="73" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E31" s="24">
         <v>11</v>
@@ -4426,16 +4423,16 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C32" s="73" t="s">
         <v>174</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C32" s="73" t="s">
-        <v>175</v>
-      </c>
       <c r="D32" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E32" s="24">
         <v>8</v>
@@ -4451,16 +4448,16 @@
     </row>
     <row r="33" spans="1:13" ht="15" thickBot="1">
       <c r="A33" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C33" s="74" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E33" s="23">
         <v>9</v>
@@ -4974,7 +4971,7 @@
         <v>70</v>
       </c>
       <c r="B64" s="43" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C64" s="79">
         <v>2</v>
@@ -4994,7 +4991,7 @@
         <v>70</v>
       </c>
       <c r="B65" s="43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C65" s="79">
         <v>3</v>
@@ -5014,7 +5011,7 @@
         <v>70</v>
       </c>
       <c r="B66" s="43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C66" s="80">
         <v>4</v>
@@ -5034,7 +5031,7 @@
         <v>70</v>
       </c>
       <c r="B67" s="43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C67" s="80">
         <v>5</v>
@@ -5054,7 +5051,7 @@
         <v>70</v>
       </c>
       <c r="B68" s="43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C68" s="80">
         <v>6</v>
@@ -5074,7 +5071,7 @@
         <v>70</v>
       </c>
       <c r="B69" s="43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C69" s="80">
         <v>8</v>
@@ -5126,7 +5123,7 @@
         <v>79</v>
       </c>
       <c r="B72" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C72" s="80">
         <v>1</v>
@@ -5144,7 +5141,7 @@
         <v>79</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C73" s="71">
         <v>2</v>
@@ -5173,7 +5170,7 @@
       <c r="K74" s="61"/>
       <c r="L74"/>
       <c r="M74" s="92" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N74" s="93"/>
       <c r="O74" s="94"/>
@@ -5183,7 +5180,7 @@
         <v>79</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C75" s="71">
         <v>4</v>
@@ -5196,7 +5193,7 @@
       <c r="K75" s="61"/>
       <c r="L75"/>
       <c r="M75" s="95" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N75" s="39"/>
       <c r="O75" s="96"/>
@@ -5206,7 +5203,7 @@
         <v>79</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C76" s="71">
         <v>5</v>
@@ -5219,7 +5216,7 @@
       <c r="K76" s="61"/>
       <c r="L76"/>
       <c r="M76" s="95" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N76" s="39"/>
       <c r="O76" s="96"/>
@@ -5229,7 +5226,7 @@
         <v>79</v>
       </c>
       <c r="B77" s="91" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C77" s="71">
         <v>6</v>
@@ -5242,7 +5239,7 @@
       <c r="K77" s="61"/>
       <c r="L77"/>
       <c r="M77" s="95" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N77" s="39"/>
       <c r="O77" s="96"/>
@@ -5252,7 +5249,7 @@
         <v>79</v>
       </c>
       <c r="B78" s="91" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C78" s="71">
         <v>7</v>
@@ -5265,7 +5262,7 @@
       <c r="K78" s="61"/>
       <c r="L78"/>
       <c r="M78" s="95" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N78" s="10"/>
       <c r="O78" s="96"/>
@@ -5275,7 +5272,7 @@
         <v>79</v>
       </c>
       <c r="B79" s="91" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C79" s="71">
         <v>8</v>
@@ -5288,7 +5285,7 @@
       <c r="K79" s="61"/>
       <c r="L79"/>
       <c r="M79" s="95" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N79" s="10"/>
       <c r="O79" s="96"/>
@@ -5298,7 +5295,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="91" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C80" s="71">
         <v>9</v>
@@ -5311,7 +5308,7 @@
       <c r="K80" s="61"/>
       <c r="L80"/>
       <c r="M80" s="95" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N80" s="10"/>
       <c r="O80" s="96"/>
@@ -5321,7 +5318,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="91" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C81" s="71">
         <v>10</v>
@@ -5334,7 +5331,7 @@
       <c r="K81" s="61"/>
       <c r="L81"/>
       <c r="M81" s="95" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N81" s="52"/>
       <c r="O81" s="96"/>
@@ -5344,7 +5341,7 @@
         <v>79</v>
       </c>
       <c r="B82" s="91" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C82" s="71">
         <v>1</v>
@@ -5357,7 +5354,7 @@
       <c r="K82" s="61"/>
       <c r="L82"/>
       <c r="M82" s="95" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N82" s="39"/>
       <c r="O82" s="96"/>
@@ -5367,7 +5364,7 @@
         <v>79</v>
       </c>
       <c r="B83" s="91" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C83" s="71">
         <v>3</v>
@@ -5380,7 +5377,7 @@
       <c r="K83" s="61"/>
       <c r="L83"/>
       <c r="M83" s="95" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N83" s="39"/>
       <c r="O83" s="96"/>
@@ -5397,7 +5394,7 @@
       <c r="K84" s="61"/>
       <c r="L84"/>
       <c r="M84" s="95" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N84" s="65"/>
       <c r="O84" s="96"/>

</xml_diff>

<commit_message>
added a ball shooter command and subsytem from old leia code
</commit_message>
<xml_diff>
--- a/documentations/2022 coordination sheet.xlsx
+++ b/documentations/2022 coordination sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minni\Documents\GitHub\2022_prod_robot\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEECA148-30E5-42B6-B978-BF5804F3612B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C313485-79E1-4B21-A55A-193B99B45E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="224">
   <si>
     <t>Relay Function Chart</t>
   </si>
@@ -963,6 +963,42 @@
   </si>
   <si>
     <t>PDP 10</t>
+  </si>
+  <si>
+    <t>Ball Shooter Bottom</t>
+  </si>
+  <si>
+    <t>Ball Shooter Top</t>
+  </si>
+  <si>
+    <t>Ball Shooter Tiny wheels</t>
+  </si>
+  <si>
+    <t>(p)775</t>
+  </si>
+  <si>
+    <t>Some encoder thingy</t>
+  </si>
+  <si>
+    <t>ID - 6</t>
+  </si>
+  <si>
+    <t>ID-13</t>
+  </si>
+  <si>
+    <t>ID-14</t>
+  </si>
+  <si>
+    <t>PDP 18</t>
+  </si>
+  <si>
+    <t>PDP 15</t>
+  </si>
+  <si>
+    <t>PDP 14</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1637,7 +1673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1969,6 +2005,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2000,13 +2048,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>417635</xdr:colOff>
-      <xdr:row>103</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>3395</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2043,13 +2091,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2065,7 +2113,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12161519" y="9618346"/>
+          <a:off x="12161519" y="10166986"/>
           <a:ext cx="1781176" cy="1655445"/>
           <a:chOff x="10410824" y="9220200"/>
           <a:chExt cx="1771651" cy="1933575"/>
@@ -3558,10 +3606,10 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:O107"/>
+  <dimension ref="A1:O110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3660,7 +3708,7 @@
         <v>8</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>119</v>
+        <v>220</v>
       </c>
       <c r="I5" s="102">
         <v>40</v>
@@ -3871,42 +3919,42 @@
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:13" s="111" customFormat="1">
+      <c r="A11" s="105" t="s">
         <v>183</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="106" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="71" t="s">
+      <c r="C11" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="108" t="s">
         <v>209</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="109" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="109" t="s">
         <v>116</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="109" t="s">
         <v>211</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="109">
         <v>30</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="106" t="s">
         <v>169</v>
       </c>
-      <c r="L11" s="10"/>
-      <c r="M11" s="4"/>
+      <c r="L11" s="109"/>
+      <c r="M11" s="110"/>
     </row>
     <row r="12" spans="1:13" s="111" customFormat="1">
       <c r="A12" s="105" t="s">
@@ -4013,36 +4061,30 @@
       <c r="L14" s="10"/>
       <c r="M14" s="33"/>
     </row>
-    <row r="15" spans="1:13" ht="24">
+    <row r="15" spans="1:13">
       <c r="A15" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="B15" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="B15" s="101" t="s">
         <v>108</v>
       </c>
       <c r="C15" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>109</v>
-      </c>
+      <c r="D15" s="17"/>
       <c r="E15" s="32" t="s">
         <v>108</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="G15" s="32" t="s">
-        <v>130</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="G15" s="32"/>
       <c r="H15" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="I15" s="103">
-        <v>40</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="I15" s="32"/>
       <c r="J15" s="32" t="s">
-        <v>10</v>
+        <v>223</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>169</v>
@@ -4052,260 +4094,284 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>195</v>
+        <v>213</v>
+      </c>
+      <c r="B16" s="101" t="s">
+        <v>108</v>
       </c>
       <c r="C16" s="71" t="s">
-        <v>196</v>
+        <v>25</v>
       </c>
       <c r="D16" s="17"/>
-      <c r="E16" s="32"/>
+      <c r="E16" s="32" t="s">
+        <v>108</v>
+      </c>
       <c r="F16" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="G16" s="32" t="s">
-        <v>198</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="G16" s="32"/>
       <c r="H16" s="32" t="s">
-        <v>196</v>
-      </c>
-      <c r="I16" s="103"/>
+        <v>222</v>
+      </c>
+      <c r="I16" s="32"/>
       <c r="J16" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="K16" s="12"/>
+        <v>223</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>169</v>
+      </c>
       <c r="L16" s="10"/>
       <c r="M16" s="33"/>
     </row>
-    <row r="17" spans="1:13" ht="24.6" thickBot="1">
-      <c r="A17" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>108</v>
+    <row r="17" spans="1:13">
+      <c r="A17" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="B17" s="101" t="s">
+        <v>215</v>
       </c>
       <c r="C17" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="17"/>
+      <c r="E17" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="L17" s="10"/>
+      <c r="M17" s="33"/>
+    </row>
+    <row r="18" spans="1:13" ht="24">
+      <c r="A18" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E18" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="F17" s="39" t="s">
+      <c r="F18" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="I18" s="103">
+        <v>40</v>
+      </c>
+      <c r="J18" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="L18" s="10"/>
+      <c r="M18" s="33"/>
+    </row>
+    <row r="19" spans="1:13" s="111" customFormat="1">
+      <c r="A19" s="114" t="s">
+        <v>194</v>
+      </c>
+      <c r="B19" s="115" t="s">
+        <v>195</v>
+      </c>
+      <c r="C19" s="107" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="108"/>
+      <c r="E19" s="115"/>
+      <c r="F19" s="109" t="s">
+        <v>197</v>
+      </c>
+      <c r="G19" s="115" t="s">
+        <v>198</v>
+      </c>
+      <c r="H19" s="115" t="s">
+        <v>196</v>
+      </c>
+      <c r="I19" s="116"/>
+      <c r="J19" s="115" t="s">
+        <v>120</v>
+      </c>
+      <c r="K19" s="106"/>
+      <c r="L19" s="109"/>
+      <c r="M19" s="117"/>
+    </row>
+    <row r="20" spans="1:13" ht="24.6" thickBot="1">
+      <c r="A20" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G20" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H20" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="I17" s="104">
+      <c r="I20" s="104">
         <v>40</v>
       </c>
-      <c r="J17" s="40" t="s">
+      <c r="J20" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K20" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="L17" s="10"/>
-      <c r="M17" s="29"/>
-    </row>
-    <row r="18" spans="1:13" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A18" s="65"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="100"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="89"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="89"/>
-      <c r="J18" s="89"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="65"/>
-      <c r="M18" s="65"/>
-    </row>
-    <row r="19" spans="1:13" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A19" s="65"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="89"/>
-      <c r="J19" s="89"/>
-      <c r="K19" s="67"/>
-      <c r="L19" s="65"/>
-      <c r="M19" s="65"/>
-    </row>
-    <row r="20" spans="1:13" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A20" s="2" t="s">
+      <c r="L20" s="10"/>
+      <c r="M20" s="29"/>
+    </row>
+    <row r="21" spans="1:13" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A21" s="65"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="89"/>
+      <c r="J21" s="89"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="65"/>
+      <c r="M21" s="65"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A22" s="65"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="100"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="89"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="89"/>
+      <c r="J22" s="89"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="65"/>
+      <c r="M22" s="65"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="1:13" s="16" customFormat="1" ht="74.400000000000006" thickTop="1">
-      <c r="A21" s="7" t="s">
+      <c r="E23" s="25"/>
+    </row>
+    <row r="24" spans="1:13" s="16" customFormat="1" ht="74.400000000000006" thickTop="1">
+      <c r="A24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B24" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="70" t="s">
+      <c r="C24" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="66" t="s">
+      <c r="E24" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F24" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H24" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="I24" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="9" t="s">
+      <c r="J24" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K21" s="26" t="s">
+      <c r="K24" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="L21" s="9" t="s">
+      <c r="L24" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="M21" s="21" t="s">
+      <c r="M24" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="3" t="s">
+    <row r="25" spans="1:13">
+      <c r="A25" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B25" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="73"/>
-      <c r="D22" s="10" t="s">
+      <c r="C25" s="73"/>
+      <c r="D25" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E25" s="24">
         <v>2</v>
       </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="C23" s="73" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="24">
-        <v>10</v>
-      </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="22"/>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="73" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="24">
-        <v>3</v>
-      </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="83" t="s">
-        <v>122</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="C25" s="73" t="s">
-        <v>124</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="E25" s="24">
-        <v>4</v>
-      </c>
-      <c r="F25" s="3"/>
+      <c r="F25" s="14"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
       <c r="K25" s="12"/>
       <c r="L25" s="10"/>
-      <c r="M25" s="22"/>
+      <c r="M25" s="22" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="83" t="s">
-        <v>126</v>
+      <c r="A26" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>127</v>
+        <v>200</v>
       </c>
       <c r="C26" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>129</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D26" s="10"/>
       <c r="E26" s="24">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="10"/>
@@ -4318,19 +4384,17 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="3" t="s">
-        <v>164</v>
+        <v>202</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>166</v>
+        <v>67</v>
       </c>
       <c r="C27" s="73" t="s">
-        <v>165</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>167</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D27" s="10"/>
       <c r="E27" s="24">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="10"/>
@@ -4339,25 +4403,27 @@
       <c r="J27" s="10"/>
       <c r="K27" s="12"/>
       <c r="L27" s="10"/>
-      <c r="M27" s="22"/>
+      <c r="M27" s="22" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="3" t="s">
-        <v>159</v>
+      <c r="A28" s="83" t="s">
+        <v>122</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>166</v>
+        <v>123</v>
       </c>
       <c r="C28" s="73" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E28" s="36">
-        <v>7</v>
-      </c>
-      <c r="F28" s="14"/>
+        <v>125</v>
+      </c>
+      <c r="E28" s="24">
+        <v>4</v>
+      </c>
+      <c r="F28" s="3"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
@@ -4366,12 +4432,22 @@
       <c r="L28" s="10"/>
       <c r="M28" s="22"/>
     </row>
-    <row r="29" spans="1:13" hidden="1">
-      <c r="A29" s="3"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="73"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="24"/>
+    <row r="29" spans="1:13">
+      <c r="A29" s="83" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" s="24">
+        <v>5</v>
+      </c>
       <c r="F29" s="14"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
@@ -4381,12 +4457,22 @@
       <c r="L29" s="10"/>
       <c r="M29" s="22"/>
     </row>
-    <row r="30" spans="1:13" hidden="1">
-      <c r="A30" s="3"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="73"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="24"/>
+    <row r="30" spans="1:13">
+      <c r="A30" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="73" t="s">
+        <v>165</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E30" s="24">
+        <v>6</v>
+      </c>
       <c r="F30" s="14"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
@@ -4398,19 +4484,19 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
-        <v>201</v>
+        <v>159</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>203</v>
+        <v>166</v>
       </c>
       <c r="C31" s="73" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="E31" s="24">
-        <v>11</v>
+        <v>168</v>
+      </c>
+      <c r="E31" s="36">
+        <v>7</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="10"/>
@@ -4421,22 +4507,12 @@
       <c r="L31" s="10"/>
       <c r="M31" s="22"/>
     </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="C32" s="73" t="s">
-        <v>174</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="E32" s="24">
-        <v>8</v>
-      </c>
+    <row r="32" spans="1:13" hidden="1">
+      <c r="A32" s="3"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="24"/>
       <c r="F32" s="14"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
@@ -4444,150 +4520,155 @@
       <c r="J32" s="10"/>
       <c r="K32" s="12"/>
       <c r="L32" s="10"/>
-      <c r="M32" s="48"/>
-    </row>
-    <row r="33" spans="1:13" ht="15" thickBot="1">
-      <c r="A33" s="5" t="s">
+      <c r="M32" s="22"/>
+    </row>
+    <row r="33" spans="1:13" hidden="1">
+      <c r="A33" s="3"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="73"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="22"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C34" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="E34" s="24">
+        <v>11</v>
+      </c>
+      <c r="F34" s="14"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="22"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C35" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="E35" s="24">
+        <v>8</v>
+      </c>
+      <c r="F35" s="14"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="48"/>
+    </row>
+    <row r="36" spans="1:13" ht="15" thickBot="1">
+      <c r="A36" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B36" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="C33" s="74" t="s">
+      <c r="C36" s="74" t="s">
         <v>175</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D36" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E36" s="23">
         <v>9</v>
       </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="23"/>
-    </row>
-    <row r="34" spans="1:13" ht="15" hidden="1" thickTop="1">
-      <c r="D34" s="1"/>
-      <c r="L34" s="65"/>
-    </row>
-    <row r="35" spans="1:13" ht="15" hidden="1" thickBot="1">
-      <c r="A35" s="2" t="s">
+      <c r="F36" s="15"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="23"/>
+    </row>
+    <row r="37" spans="1:13" ht="15" hidden="1" thickTop="1">
+      <c r="D37" s="1"/>
+      <c r="L37" s="65"/>
+    </row>
+    <row r="38" spans="1:13" ht="15" hidden="1" thickBot="1">
+      <c r="A38" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E35" s="18"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="28"/>
-    </row>
-    <row r="36" spans="1:13" ht="84.6" hidden="1" thickTop="1">
-      <c r="A36" s="20" t="s">
+      <c r="E38" s="18"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="28"/>
+    </row>
+    <row r="39" spans="1:13" ht="84.6" hidden="1" thickTop="1">
+      <c r="A39" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="70" t="s">
+      <c r="C39" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D39" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E39" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="9" t="s">
+      <c r="F39" s="8"/>
+      <c r="G39" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="H36" s="9"/>
-      <c r="I36" s="26" t="s">
+      <c r="H39" s="9"/>
+      <c r="I39" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="J36" s="8" t="s">
+      <c r="J39" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K36" s="8" t="s">
+      <c r="K39" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L36" s="30"/>
-    </row>
-    <row r="37" spans="1:13" hidden="1">
-      <c r="A37" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="12"/>
-      <c r="C37" s="71"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="4"/>
-    </row>
-    <row r="38" spans="1:13" hidden="1">
-      <c r="A38" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="12"/>
-      <c r="C38" s="71"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="4"/>
-    </row>
-    <row r="39" spans="1:13" hidden="1">
-      <c r="A39" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="71"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="4"/>
+      <c r="L39" s="30"/>
     </row>
     <row r="40" spans="1:13" hidden="1">
       <c r="A40" s="3" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="B40" s="12"/>
       <c r="C40" s="71"/>
       <c r="D40" s="12"/>
       <c r="E40" s="12" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F40" s="10"/>
       <c r="G40" s="10" t="s">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
@@ -4597,17 +4678,17 @@
     </row>
     <row r="41" spans="1:13" hidden="1">
       <c r="A41" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" s="10"/>
+        <v>53</v>
+      </c>
+      <c r="B41" s="12"/>
       <c r="C41" s="71"/>
       <c r="D41" s="12"/>
       <c r="E41" s="12" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="10" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
@@ -4617,17 +4698,17 @@
     </row>
     <row r="42" spans="1:13" hidden="1">
       <c r="A42" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B42" s="10"/>
+        <v>89</v>
+      </c>
+      <c r="B42" s="12"/>
       <c r="C42" s="71"/>
       <c r="D42" s="12"/>
       <c r="E42" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
@@ -4636,118 +4717,132 @@
       <c r="L42" s="4"/>
     </row>
     <row r="43" spans="1:13" hidden="1">
-      <c r="A43" s="3"/>
-      <c r="B43" s="10"/>
+      <c r="A43" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="12"/>
       <c r="C43" s="71"/>
       <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
+      <c r="E43" s="12" t="s">
+        <v>94</v>
+      </c>
       <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
+      <c r="G43" s="10" t="s">
+        <v>97</v>
+      </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10"/>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
       <c r="L43" s="4"/>
     </row>
-    <row r="44" spans="1:13" ht="15" hidden="1" thickBot="1">
-      <c r="A44" s="3"/>
+    <row r="44" spans="1:13" hidden="1">
+      <c r="A44" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="B44" s="10"/>
       <c r="C44" s="71"/>
       <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
+      <c r="E44" s="12" t="s">
+        <v>95</v>
+      </c>
       <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
+      <c r="G44" s="10" t="s">
+        <v>98</v>
+      </c>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
       <c r="L44" s="4"/>
     </row>
-    <row r="45" spans="1:13" ht="15.6" hidden="1" thickTop="1" thickBot="1">
-      <c r="A45" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E45" s="18"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="25"/>
-    </row>
-    <row r="46" spans="1:13" ht="101.4" hidden="1" thickTop="1">
-      <c r="A46" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" s="70" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F46" s="8"/>
-      <c r="G46" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H46" s="9"/>
-      <c r="I46" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="J46" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K46" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L46" s="30"/>
-    </row>
-    <row r="47" spans="1:13" hidden="1">
+    <row r="45" spans="1:13" hidden="1">
+      <c r="A45" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="4"/>
+    </row>
+    <row r="46" spans="1:13" hidden="1">
+      <c r="A46" s="3"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="4"/>
+    </row>
+    <row r="47" spans="1:13" ht="15" hidden="1" thickBot="1">
       <c r="A47" s="3"/>
-      <c r="B47" s="12"/>
+      <c r="B47" s="10"/>
       <c r="C47" s="71"/>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="10"/>
-      <c r="G47" s="10" t="s">
-        <v>60</v>
-      </c>
+      <c r="G47" s="10"/>
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
-      <c r="J47" s="10">
-        <v>12</v>
-      </c>
+      <c r="J47" s="10"/>
       <c r="K47" s="10"/>
       <c r="L47" s="4"/>
     </row>
-    <row r="48" spans="1:13" hidden="1">
-      <c r="A48" s="3"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="71"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="84"/>
-      <c r="F48" s="86"/>
-      <c r="G48" s="86"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
-      <c r="L48" s="4"/>
-    </row>
-    <row r="49" spans="1:14" hidden="1">
-      <c r="A49" s="83"/>
-      <c r="B49" s="86"/>
-      <c r="C49" s="85"/>
-      <c r="D49" s="84"/>
-      <c r="E49" s="84"/>
-      <c r="F49" s="86"/>
-      <c r="G49" s="86"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-      <c r="L49" s="4"/>
+    <row r="48" spans="1:13" ht="15.6" hidden="1" thickTop="1" thickBot="1">
+      <c r="A48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="18"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="25"/>
+    </row>
+    <row r="49" spans="1:14" ht="101.4" hidden="1" thickTop="1">
+      <c r="A49" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F49" s="8"/>
+      <c r="G49" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H49" s="9"/>
+      <c r="I49" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="J49" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K49" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L49" s="30"/>
     </row>
     <row r="50" spans="1:14" hidden="1">
       <c r="A50" s="3"/>
@@ -4756,21 +4851,25 @@
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
+      <c r="G50" s="10" t="s">
+        <v>60</v>
+      </c>
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
+      <c r="J50" s="10">
+        <v>12</v>
+      </c>
       <c r="K50" s="10"/>
       <c r="L50" s="4"/>
     </row>
     <row r="51" spans="1:14" hidden="1">
       <c r="A51" s="3"/>
-      <c r="B51" s="10"/>
+      <c r="B51" s="12"/>
       <c r="C51" s="71"/>
       <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
+      <c r="E51" s="84"/>
+      <c r="F51" s="86"/>
+      <c r="G51" s="86"/>
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
       <c r="J51" s="10"/>
@@ -4778,13 +4877,13 @@
       <c r="L51" s="4"/>
     </row>
     <row r="52" spans="1:14" hidden="1">
-      <c r="A52" s="3"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="71"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
+      <c r="A52" s="83"/>
+      <c r="B52" s="86"/>
+      <c r="C52" s="85"/>
+      <c r="D52" s="84"/>
+      <c r="E52" s="84"/>
+      <c r="F52" s="86"/>
+      <c r="G52" s="86"/>
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
       <c r="J52" s="10"/>
@@ -4793,7 +4892,7 @@
     </row>
     <row r="53" spans="1:14" hidden="1">
       <c r="A53" s="3"/>
-      <c r="B53" s="10"/>
+      <c r="B53" s="12"/>
       <c r="C53" s="71"/>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
@@ -4819,210 +4918,192 @@
       <c r="K54" s="10"/>
       <c r="L54" s="4"/>
     </row>
-    <row r="55" spans="1:14" ht="15" hidden="1" thickBot="1">
-      <c r="A55" s="5"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="72"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11"/>
-      <c r="L55" s="6"/>
-    </row>
-    <row r="56" spans="1:14" ht="15" thickTop="1"/>
-    <row r="58" spans="1:14" ht="15" thickBot="1">
-      <c r="A58"/>
-      <c r="B58"/>
-      <c r="C58" s="75"/>
-      <c r="D58"/>
-      <c r="E58" s="53"/>
-      <c r="F58"/>
-      <c r="G58"/>
-      <c r="H58"/>
-      <c r="I58"/>
-      <c r="J58"/>
-      <c r="K58"/>
-      <c r="L58"/>
-      <c r="M58"/>
-      <c r="N58"/>
-    </row>
-    <row r="59" spans="1:14" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A59" s="42" t="s">
+    <row r="55" spans="1:14" hidden="1">
+      <c r="A55" s="3"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="71"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="10"/>
+      <c r="K55" s="10"/>
+      <c r="L55" s="4"/>
+    </row>
+    <row r="56" spans="1:14" hidden="1">
+      <c r="A56" s="3"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="10"/>
+      <c r="L56" s="4"/>
+    </row>
+    <row r="57" spans="1:14" hidden="1">
+      <c r="A57" s="3"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="71"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="10"/>
+      <c r="L57" s="4"/>
+    </row>
+    <row r="58" spans="1:14" ht="15" hidden="1" thickBot="1">
+      <c r="A58" s="5"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="72"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="6"/>
+    </row>
+    <row r="59" spans="1:14" ht="15" thickTop="1"/>
+    <row r="61" spans="1:14" ht="15" thickBot="1">
+      <c r="A61"/>
+      <c r="B61"/>
+      <c r="C61" s="75"/>
+      <c r="D61"/>
+      <c r="E61" s="53"/>
+      <c r="F61"/>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61"/>
+      <c r="J61"/>
+      <c r="K61"/>
+      <c r="L61"/>
+      <c r="M61"/>
+      <c r="N61"/>
+    </row>
+    <row r="62" spans="1:14" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A62" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="B59" s="25"/>
-      <c r="C59" s="76"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="25"/>
-      <c r="F59" s="25"/>
-      <c r="G59" s="25"/>
-      <c r="H59" s="25"/>
-      <c r="I59" s="25"/>
-      <c r="J59" s="25"/>
-      <c r="K59" s="58"/>
-      <c r="L59"/>
-    </row>
-    <row r="60" spans="1:14" ht="15" thickTop="1">
-      <c r="A60" s="8" t="s">
+      <c r="B62" s="25"/>
+      <c r="C62" s="76"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="25"/>
+      <c r="H62" s="25"/>
+      <c r="I62" s="25"/>
+      <c r="J62" s="25"/>
+      <c r="K62" s="58"/>
+      <c r="L62"/>
+    </row>
+    <row r="63" spans="1:14" ht="15" thickTop="1">
+      <c r="A63" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B63" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C60" s="68" t="s">
+      <c r="C63" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="D63" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="E63" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F60" s="8" t="s">
+      <c r="F63" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G60" s="46" t="s">
+      <c r="G63" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="H60" s="8" t="s">
+      <c r="H63" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="I60" s="8"/>
-      <c r="J60" s="8"/>
-      <c r="K60" s="59"/>
-      <c r="L60"/>
-    </row>
-    <row r="61" spans="1:14" ht="28.8">
-      <c r="A61" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B61" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="C61" s="77" t="s">
-        <v>71</v>
-      </c>
-      <c r="D61" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="E61" s="54"/>
-      <c r="F61" s="45"/>
-      <c r="G61" s="45"/>
-      <c r="H61" s="45"/>
-      <c r="I61" s="45"/>
-      <c r="J61" s="45"/>
-      <c r="K61" s="60"/>
-      <c r="L61" s="112" t="s">
-        <v>75</v>
-      </c>
-      <c r="M61" s="113" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="28.8">
-      <c r="A62" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B62" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C62" s="78" t="s">
-        <v>27</v>
-      </c>
-      <c r="D62" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="E62" s="34"/>
-      <c r="F62" s="39"/>
-      <c r="G62" s="39"/>
-      <c r="H62" s="39"/>
-      <c r="I62" s="39"/>
-      <c r="J62" s="39"/>
-      <c r="K62" s="61"/>
-      <c r="L62" s="112"/>
-      <c r="M62" s="113"/>
-    </row>
-    <row r="63" spans="1:14">
-      <c r="A63" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B63" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="C63" s="78">
-        <v>1</v>
-      </c>
-      <c r="D63" s="50"/>
-      <c r="E63" s="39"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="56"/>
-      <c r="H63" s="39"/>
-      <c r="I63" s="39"/>
-      <c r="J63" s="51"/>
-      <c r="K63" s="61"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8"/>
+      <c r="K63" s="59"/>
       <c r="L63"/>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" ht="28.8">
       <c r="A64" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="B64" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="C64" s="79">
-        <v>2</v>
-      </c>
-      <c r="D64" s="50"/>
+      <c r="B64" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C64" s="77" t="s">
+        <v>71</v>
+      </c>
+      <c r="D64" s="63" t="s">
+        <v>72</v>
+      </c>
       <c r="E64" s="54"/>
-      <c r="F64" s="43"/>
-      <c r="G64" s="39"/>
-      <c r="H64" s="39"/>
-      <c r="I64" s="39"/>
-      <c r="J64" s="39"/>
-      <c r="K64" s="61"/>
-      <c r="L64"/>
-    </row>
-    <row r="65" spans="1:15">
+      <c r="F64" s="45"/>
+      <c r="G64" s="45"/>
+      <c r="H64" s="45"/>
+      <c r="I64" s="45"/>
+      <c r="J64" s="45"/>
+      <c r="K64" s="60"/>
+      <c r="L64" s="112" t="s">
+        <v>75</v>
+      </c>
+      <c r="M64" s="113" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" ht="28.8">
       <c r="A65" s="41" t="s">
         <v>70</v>
       </c>
       <c r="B65" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="C65" s="79">
-        <v>3</v>
-      </c>
-      <c r="D65" s="50"/>
-      <c r="E65" s="54"/>
-      <c r="F65" s="43"/>
+        <v>45</v>
+      </c>
+      <c r="C65" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="D65" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="E65" s="34"/>
+      <c r="F65" s="39"/>
       <c r="G65" s="39"/>
       <c r="H65" s="39"/>
       <c r="I65" s="39"/>
       <c r="J65" s="39"/>
       <c r="K65" s="61"/>
-      <c r="L65"/>
+      <c r="L65" s="112"/>
+      <c r="M65" s="113"/>
     </row>
     <row r="66" spans="1:15">
       <c r="A66" s="41" t="s">
         <v>70</v>
       </c>
       <c r="B66" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="C66" s="80">
-        <v>4</v>
+        <v>74</v>
+      </c>
+      <c r="C66" s="78">
+        <v>1</v>
       </c>
       <c r="D66" s="50"/>
-      <c r="E66" s="54"/>
+      <c r="E66" s="39"/>
       <c r="F66" s="43"/>
-      <c r="G66" s="39"/>
+      <c r="G66" s="56"/>
       <c r="H66" s="39"/>
       <c r="I66" s="39"/>
-      <c r="J66" s="39"/>
+      <c r="J66" s="51"/>
       <c r="K66" s="61"/>
       <c r="L66"/>
     </row>
@@ -5031,10 +5112,10 @@
         <v>70</v>
       </c>
       <c r="B67" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="C67" s="80">
-        <v>5</v>
+        <v>131</v>
+      </c>
+      <c r="C67" s="79">
+        <v>2</v>
       </c>
       <c r="D67" s="50"/>
       <c r="E67" s="54"/>
@@ -5044,22 +5125,22 @@
       <c r="I67" s="39"/>
       <c r="J67" s="39"/>
       <c r="K67" s="61"/>
-      <c r="L67" s="44"/>
+      <c r="L67"/>
     </row>
     <row r="68" spans="1:15">
       <c r="A68" s="41" t="s">
         <v>70</v>
       </c>
       <c r="B68" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="C68" s="80">
-        <v>6</v>
+        <v>132</v>
+      </c>
+      <c r="C68" s="79">
+        <v>3</v>
       </c>
       <c r="D68" s="50"/>
-      <c r="E68" s="39"/>
-      <c r="F68" s="10"/>
-      <c r="G68" s="10"/>
+      <c r="E68" s="54"/>
+      <c r="F68" s="43"/>
+      <c r="G68" s="39"/>
       <c r="H68" s="39"/>
       <c r="I68" s="39"/>
       <c r="J68" s="39"/>
@@ -5071,15 +5152,15 @@
         <v>70</v>
       </c>
       <c r="B69" s="43" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C69" s="80">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D69" s="50"/>
-      <c r="E69" s="34"/>
-      <c r="F69" s="34"/>
-      <c r="G69" s="10"/>
+      <c r="E69" s="54"/>
+      <c r="F69" s="43"/>
+      <c r="G69" s="39"/>
       <c r="H69" s="39"/>
       <c r="I69" s="39"/>
       <c r="J69" s="39"/>
@@ -5090,204 +5171,195 @@
       <c r="A70" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="B70" s="43"/>
-      <c r="C70" s="80"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="39"/>
-      <c r="F70" s="39"/>
-      <c r="G70" s="41"/>
+      <c r="B70" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="C70" s="80">
+        <v>5</v>
+      </c>
+      <c r="D70" s="50"/>
+      <c r="E70" s="54"/>
+      <c r="F70" s="43"/>
+      <c r="G70" s="39"/>
       <c r="H70" s="39"/>
       <c r="I70" s="39"/>
       <c r="J70" s="39"/>
       <c r="K70" s="61"/>
-      <c r="L70"/>
-      <c r="M70" s="2"/>
-      <c r="N70" s="2"/>
+      <c r="L70" s="44"/>
     </row>
     <row r="71" spans="1:15">
-      <c r="A71" s="41"/>
-      <c r="B71" s="43"/>
-      <c r="C71" s="80"/>
-      <c r="D71" s="39"/>
+      <c r="A71" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="C71" s="80">
+        <v>6</v>
+      </c>
+      <c r="D71" s="50"/>
       <c r="E71" s="39"/>
-      <c r="F71" s="39"/>
-      <c r="G71" s="39"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
       <c r="H71" s="39"/>
       <c r="I71" s="39"/>
       <c r="J71" s="39"/>
       <c r="K71" s="61"/>
       <c r="L71"/>
     </row>
-    <row r="72" spans="1:15" ht="15.6">
+    <row r="72" spans="1:15">
       <c r="A72" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B72" s="39" t="s">
-        <v>153</v>
+        <v>70</v>
+      </c>
+      <c r="B72" s="43" t="s">
+        <v>136</v>
       </c>
       <c r="C72" s="80">
-        <v>1</v>
-      </c>
-      <c r="D72" s="34"/>
-      <c r="E72" s="39"/>
-      <c r="H72" s="90"/>
+        <v>8</v>
+      </c>
+      <c r="D72" s="50"/>
+      <c r="E72" s="34"/>
+      <c r="F72" s="34"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="39"/>
       <c r="I72" s="39"/>
       <c r="J72" s="39"/>
       <c r="K72" s="61"/>
       <c r="L72"/>
     </row>
-    <row r="73" spans="1:15" ht="16.2" thickBot="1">
+    <row r="73" spans="1:15">
       <c r="A73" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C73" s="71">
-        <v>2</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B73" s="43"/>
+      <c r="C73" s="80"/>
       <c r="D73" s="39"/>
-      <c r="E73" s="57"/>
-      <c r="H73" s="90"/>
+      <c r="E73" s="39"/>
+      <c r="F73" s="39"/>
+      <c r="G73" s="41"/>
+      <c r="H73" s="39"/>
       <c r="I73" s="39"/>
       <c r="J73" s="39"/>
       <c r="K73" s="61"/>
       <c r="L73"/>
-    </row>
-    <row r="74" spans="1:15" ht="15.6">
-      <c r="A74" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B74" s="39"/>
-      <c r="C74" s="80">
-        <v>3</v>
-      </c>
+      <c r="M73" s="2"/>
+      <c r="N73" s="2"/>
+    </row>
+    <row r="74" spans="1:15">
+      <c r="A74" s="41"/>
+      <c r="B74" s="43"/>
+      <c r="C74" s="80"/>
       <c r="D74" s="39"/>
-      <c r="E74" s="38"/>
-      <c r="H74" s="90"/>
+      <c r="E74" s="39"/>
+      <c r="F74" s="39"/>
+      <c r="G74" s="39"/>
+      <c r="H74" s="39"/>
       <c r="I74" s="39"/>
       <c r="J74" s="39"/>
       <c r="K74" s="61"/>
       <c r="L74"/>
-      <c r="M74" s="92" t="s">
-        <v>158</v>
-      </c>
-      <c r="N74" s="93"/>
-      <c r="O74" s="94"/>
     </row>
     <row r="75" spans="1:15" ht="15.6">
       <c r="A75" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="B75" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C75" s="71">
-        <v>4</v>
-      </c>
-      <c r="D75" s="39"/>
-      <c r="E75" s="55"/>
+      <c r="B75" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C75" s="80">
+        <v>1</v>
+      </c>
+      <c r="D75" s="34"/>
+      <c r="E75" s="39"/>
       <c r="H75" s="90"/>
       <c r="I75" s="39"/>
       <c r="J75" s="39"/>
       <c r="K75" s="61"/>
       <c r="L75"/>
-      <c r="M75" s="95" t="s">
-        <v>137</v>
-      </c>
-      <c r="N75" s="39"/>
-      <c r="O75" s="96"/>
-    </row>
-    <row r="76" spans="1:15" ht="15.6">
+    </row>
+    <row r="76" spans="1:15" ht="16.2" thickBot="1">
       <c r="A76" s="41" t="s">
         <v>79</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C76" s="71">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D76" s="39"/>
-      <c r="E76" s="55"/>
+      <c r="E76" s="57"/>
       <c r="H76" s="90"/>
       <c r="I76" s="39"/>
       <c r="J76" s="39"/>
       <c r="K76" s="61"/>
       <c r="L76"/>
-      <c r="M76" s="95" t="s">
-        <v>138</v>
-      </c>
-      <c r="N76" s="39"/>
-      <c r="O76" s="96"/>
     </row>
     <row r="77" spans="1:15" ht="15.6">
       <c r="A77" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="B77" s="91" t="s">
-        <v>150</v>
-      </c>
-      <c r="C77" s="71">
-        <v>6</v>
+      <c r="B77" s="39"/>
+      <c r="C77" s="80">
+        <v>3</v>
       </c>
       <c r="D77" s="39"/>
-      <c r="E77" s="39"/>
+      <c r="E77" s="38"/>
       <c r="H77" s="90"/>
       <c r="I77" s="39"/>
       <c r="J77" s="39"/>
       <c r="K77" s="61"/>
       <c r="L77"/>
-      <c r="M77" s="95" t="s">
-        <v>139</v>
-      </c>
-      <c r="N77" s="39"/>
-      <c r="O77" s="96"/>
+      <c r="M77" s="92" t="s">
+        <v>158</v>
+      </c>
+      <c r="N77" s="93"/>
+      <c r="O77" s="94"/>
     </row>
     <row r="78" spans="1:15" ht="15.6">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="B78" s="91" t="s">
-        <v>151</v>
+      <c r="B78" s="10" t="s">
+        <v>154</v>
       </c>
       <c r="C78" s="71">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D78" s="39"/>
-      <c r="E78" s="34"/>
+      <c r="E78" s="55"/>
       <c r="H78" s="90"/>
       <c r="I78" s="39"/>
       <c r="J78" s="39"/>
       <c r="K78" s="61"/>
       <c r="L78"/>
       <c r="M78" s="95" t="s">
-        <v>140</v>
-      </c>
-      <c r="N78" s="10"/>
+        <v>137</v>
+      </c>
+      <c r="N78" s="39"/>
       <c r="O78" s="96"/>
     </row>
     <row r="79" spans="1:15" ht="15.6">
       <c r="A79" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="B79" s="91" t="s">
-        <v>152</v>
+      <c r="B79" s="10" t="s">
+        <v>149</v>
       </c>
       <c r="C79" s="71">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D79" s="39"/>
-      <c r="E79" s="39"/>
+      <c r="E79" s="55"/>
       <c r="H79" s="90"/>
       <c r="I79" s="39"/>
       <c r="J79" s="39"/>
       <c r="K79" s="61"/>
       <c r="L79"/>
       <c r="M79" s="95" t="s">
-        <v>141</v>
-      </c>
-      <c r="N79" s="10"/>
+        <v>138</v>
+      </c>
+      <c r="N79" s="39"/>
       <c r="O79" s="96"/>
     </row>
     <row r="80" spans="1:15" ht="15.6">
@@ -5295,10 +5367,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="91" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C80" s="71">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D80" s="39"/>
       <c r="E80" s="39"/>
@@ -5308,32 +5380,32 @@
       <c r="K80" s="61"/>
       <c r="L80"/>
       <c r="M80" s="95" t="s">
-        <v>142</v>
-      </c>
-      <c r="N80" s="10"/>
+        <v>139</v>
+      </c>
+      <c r="N80" s="39"/>
       <c r="O80" s="96"/>
     </row>
     <row r="81" spans="1:15" ht="15.6">
-      <c r="A81" s="41" t="s">
+      <c r="A81" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B81" s="91" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C81" s="71">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D81" s="39"/>
-      <c r="E81" s="39"/>
+      <c r="E81" s="34"/>
       <c r="H81" s="90"/>
       <c r="I81" s="39"/>
       <c r="J81" s="39"/>
       <c r="K81" s="61"/>
       <c r="L81"/>
       <c r="M81" s="95" t="s">
-        <v>143</v>
-      </c>
-      <c r="N81" s="52"/>
+        <v>140</v>
+      </c>
+      <c r="N81" s="10"/>
       <c r="O81" s="96"/>
     </row>
     <row r="82" spans="1:15" ht="15.6">
@@ -5341,22 +5413,22 @@
         <v>79</v>
       </c>
       <c r="B82" s="91" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C82" s="71">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D82" s="39"/>
       <c r="E82" s="39"/>
-      <c r="H82" s="39"/>
+      <c r="H82" s="90"/>
       <c r="I82" s="39"/>
       <c r="J82" s="39"/>
       <c r="K82" s="61"/>
       <c r="L82"/>
       <c r="M82" s="95" t="s">
-        <v>144</v>
-      </c>
-      <c r="N82" s="39"/>
+        <v>141</v>
+      </c>
+      <c r="N82" s="10"/>
       <c r="O82" s="96"/>
     </row>
     <row r="83" spans="1:15" ht="15.6">
@@ -5364,166 +5436,187 @@
         <v>79</v>
       </c>
       <c r="B83" s="91" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C83" s="71">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D83" s="39"/>
       <c r="E83" s="39"/>
-      <c r="H83" s="39"/>
+      <c r="H83" s="90"/>
       <c r="I83" s="39"/>
       <c r="J83" s="39"/>
       <c r="K83" s="61"/>
       <c r="L83"/>
       <c r="M83" s="95" t="s">
-        <v>145</v>
-      </c>
-      <c r="N83" s="39"/>
+        <v>142</v>
+      </c>
+      <c r="N83" s="10"/>
       <c r="O83" s="96"/>
     </row>
     <row r="84" spans="1:15" ht="15.6">
-      <c r="A84" s="41"/>
-      <c r="B84" s="39"/>
-      <c r="C84" s="80"/>
+      <c r="A84" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B84" s="91" t="s">
+        <v>157</v>
+      </c>
+      <c r="C84" s="71">
+        <v>10</v>
+      </c>
       <c r="D84" s="39"/>
       <c r="E84" s="39"/>
-      <c r="H84" s="39"/>
+      <c r="H84" s="90"/>
       <c r="I84" s="39"/>
       <c r="J84" s="39"/>
       <c r="K84" s="61"/>
       <c r="L84"/>
       <c r="M84" s="95" t="s">
-        <v>146</v>
-      </c>
-      <c r="N84" s="65"/>
+        <v>143</v>
+      </c>
+      <c r="N84" s="52"/>
       <c r="O84" s="96"/>
     </row>
-    <row r="85" spans="1:15" ht="15" thickBot="1">
-      <c r="A85" s="41"/>
-      <c r="B85" s="43"/>
-      <c r="C85" s="80"/>
-      <c r="D85" s="34"/>
+    <row r="85" spans="1:15" ht="15.6">
+      <c r="A85" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B85" s="91" t="s">
+        <v>147</v>
+      </c>
+      <c r="C85" s="71">
+        <v>1</v>
+      </c>
+      <c r="D85" s="39"/>
       <c r="E85" s="39"/>
       <c r="H85" s="39"/>
       <c r="I85" s="39"/>
       <c r="J85" s="39"/>
       <c r="K85" s="61"/>
       <c r="L85"/>
-      <c r="M85" s="97"/>
-      <c r="N85" s="98"/>
-      <c r="O85" s="99"/>
-    </row>
-    <row r="86" spans="1:15" ht="15" thickBot="1">
-      <c r="A86" s="47"/>
-      <c r="B86" s="35"/>
-      <c r="C86" s="81"/>
-      <c r="D86" s="35"/>
-      <c r="E86" s="40"/>
-      <c r="F86" s="40"/>
-      <c r="G86" s="40"/>
-      <c r="H86" s="40"/>
-      <c r="I86" s="40"/>
-      <c r="J86" s="40"/>
-      <c r="K86" s="62"/>
+      <c r="M85" s="95" t="s">
+        <v>144</v>
+      </c>
+      <c r="N85" s="39"/>
+      <c r="O85" s="96"/>
+    </row>
+    <row r="86" spans="1:15" ht="15.6">
+      <c r="A86" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B86" s="91" t="s">
+        <v>148</v>
+      </c>
+      <c r="C86" s="71">
+        <v>3</v>
+      </c>
+      <c r="D86" s="39"/>
+      <c r="E86" s="39"/>
+      <c r="H86" s="39"/>
+      <c r="I86" s="39"/>
+      <c r="J86" s="39"/>
+      <c r="K86" s="61"/>
       <c r="L86"/>
-    </row>
-    <row r="87" spans="1:15" ht="15" thickTop="1">
-      <c r="A87" s="2"/>
-      <c r="D87" s="1"/>
-      <c r="K87" s="64"/>
-    </row>
-    <row r="88" spans="1:15">
-      <c r="A88" s="65"/>
-      <c r="B88" s="65"/>
-      <c r="C88" s="82"/>
-      <c r="D88" s="67"/>
-      <c r="E88" s="67"/>
-      <c r="F88" s="65"/>
-      <c r="G88" s="65"/>
-      <c r="H88" s="65"/>
-      <c r="I88" s="65"/>
-      <c r="K88" s="65"/>
-      <c r="L88" s="65"/>
-    </row>
-    <row r="89" spans="1:15">
-      <c r="A89" s="65"/>
-      <c r="B89" s="65"/>
-      <c r="C89" s="82"/>
-      <c r="D89" s="67"/>
-      <c r="E89" s="67"/>
-      <c r="F89" s="65"/>
-      <c r="G89" s="65"/>
-      <c r="H89" s="65"/>
-      <c r="I89" s="65"/>
-      <c r="J89" s="65"/>
-      <c r="K89" s="65"/>
-      <c r="L89" s="65"/>
-    </row>
-    <row r="90" spans="1:15">
-      <c r="D90" s="64"/>
-      <c r="E90" s="64"/>
-      <c r="K90" s="1"/>
-      <c r="N90"/>
+      <c r="M86" s="95" t="s">
+        <v>145</v>
+      </c>
+      <c r="N86" s="39"/>
+      <c r="O86" s="96"/>
+    </row>
+    <row r="87" spans="1:15" ht="15.6">
+      <c r="A87" s="41"/>
+      <c r="B87" s="39"/>
+      <c r="C87" s="80"/>
+      <c r="D87" s="39"/>
+      <c r="E87" s="39"/>
+      <c r="H87" s="39"/>
+      <c r="I87" s="39"/>
+      <c r="J87" s="39"/>
+      <c r="K87" s="61"/>
+      <c r="L87"/>
+      <c r="M87" s="95" t="s">
+        <v>146</v>
+      </c>
+      <c r="N87" s="65"/>
+      <c r="O87" s="96"/>
+    </row>
+    <row r="88" spans="1:15" ht="15" thickBot="1">
+      <c r="A88" s="41"/>
+      <c r="B88" s="43"/>
+      <c r="C88" s="80"/>
+      <c r="D88" s="34"/>
+      <c r="E88" s="39"/>
+      <c r="H88" s="39"/>
+      <c r="I88" s="39"/>
+      <c r="J88" s="39"/>
+      <c r="K88" s="61"/>
+      <c r="L88"/>
+      <c r="M88" s="97"/>
+      <c r="N88" s="98"/>
+      <c r="O88" s="99"/>
+    </row>
+    <row r="89" spans="1:15" ht="15" thickBot="1">
+      <c r="A89" s="47"/>
+      <c r="B89" s="35"/>
+      <c r="C89" s="81"/>
+      <c r="D89" s="35"/>
+      <c r="E89" s="40"/>
+      <c r="F89" s="40"/>
+      <c r="G89" s="40"/>
+      <c r="H89" s="40"/>
+      <c r="I89" s="40"/>
+      <c r="J89" s="40"/>
+      <c r="K89" s="62"/>
+      <c r="L89"/>
+    </row>
+    <row r="90" spans="1:15" ht="15" thickTop="1">
+      <c r="A90" s="2"/>
+      <c r="D90" s="1"/>
+      <c r="K90" s="64"/>
     </row>
     <row r="91" spans="1:15">
-      <c r="D91" s="64"/>
-      <c r="E91" s="64"/>
-      <c r="K91" s="1"/>
-      <c r="N91"/>
+      <c r="A91" s="65"/>
+      <c r="B91" s="65"/>
+      <c r="C91" s="82"/>
+      <c r="D91" s="67"/>
+      <c r="E91" s="67"/>
+      <c r="F91" s="65"/>
+      <c r="G91" s="65"/>
+      <c r="H91" s="65"/>
+      <c r="I91" s="65"/>
+      <c r="K91" s="65"/>
+      <c r="L91" s="65"/>
     </row>
     <row r="92" spans="1:15">
-      <c r="D92" s="64"/>
-      <c r="E92" s="64"/>
-      <c r="K92" s="1"/>
-      <c r="N92"/>
+      <c r="A92" s="65"/>
+      <c r="B92" s="65"/>
+      <c r="C92" s="82"/>
+      <c r="D92" s="67"/>
+      <c r="E92" s="67"/>
+      <c r="F92" s="65"/>
+      <c r="G92" s="65"/>
+      <c r="H92" s="65"/>
+      <c r="I92" s="65"/>
+      <c r="J92" s="65"/>
+      <c r="K92" s="65"/>
+      <c r="L92" s="65"/>
     </row>
     <row r="93" spans="1:15">
-      <c r="A93"/>
-      <c r="B93"/>
-      <c r="C93" s="75"/>
-      <c r="D93"/>
-      <c r="E93" s="53"/>
-      <c r="F93"/>
-      <c r="G93"/>
-      <c r="H93"/>
-      <c r="I93"/>
-      <c r="J93"/>
-      <c r="K93"/>
-      <c r="L93"/>
-      <c r="M93"/>
+      <c r="D93" s="64"/>
+      <c r="E93" s="64"/>
+      <c r="K93" s="1"/>
       <c r="N93"/>
     </row>
     <row r="94" spans="1:15">
-      <c r="A94"/>
-      <c r="B94"/>
-      <c r="C94" s="75"/>
-      <c r="D94"/>
-      <c r="E94" s="53"/>
-      <c r="F94"/>
-      <c r="G94"/>
-      <c r="H94"/>
-      <c r="I94"/>
-      <c r="J94"/>
-      <c r="K94"/>
-      <c r="L94"/>
-      <c r="M94"/>
+      <c r="D94" s="64"/>
+      <c r="E94" s="64"/>
+      <c r="K94" s="1"/>
       <c r="N94"/>
     </row>
     <row r="95" spans="1:15">
-      <c r="A95"/>
-      <c r="B95"/>
-      <c r="C95" s="75"/>
-      <c r="D95"/>
-      <c r="E95" s="53"/>
-      <c r="F95"/>
-      <c r="G95"/>
-      <c r="H95"/>
-      <c r="I95"/>
-      <c r="J95"/>
-      <c r="K95"/>
-      <c r="L95"/>
-      <c r="M95"/>
+      <c r="D95" s="64"/>
+      <c r="E95" s="64"/>
+      <c r="K95" s="1"/>
       <c r="N95"/>
     </row>
     <row r="96" spans="1:15">
@@ -5670,20 +5763,68 @@
       <c r="M104"/>
       <c r="N104"/>
     </row>
+    <row r="105" spans="1:14">
+      <c r="A105"/>
+      <c r="B105"/>
+      <c r="C105" s="75"/>
+      <c r="D105"/>
+      <c r="E105" s="53"/>
+      <c r="F105"/>
+      <c r="G105"/>
+      <c r="H105"/>
+      <c r="I105"/>
+      <c r="J105"/>
+      <c r="K105"/>
+      <c r="L105"/>
+      <c r="M105"/>
+      <c r="N105"/>
+    </row>
     <row r="106" spans="1:14">
-      <c r="A106" s="1" t="s">
+      <c r="A106"/>
+      <c r="B106"/>
+      <c r="C106" s="75"/>
+      <c r="D106"/>
+      <c r="E106" s="53"/>
+      <c r="F106"/>
+      <c r="G106"/>
+      <c r="H106"/>
+      <c r="I106"/>
+      <c r="J106"/>
+      <c r="K106"/>
+      <c r="L106"/>
+      <c r="M106"/>
+      <c r="N106"/>
+    </row>
+    <row r="107" spans="1:14">
+      <c r="A107"/>
+      <c r="B107"/>
+      <c r="C107" s="75"/>
+      <c r="D107"/>
+      <c r="E107" s="53"/>
+      <c r="F107"/>
+      <c r="G107"/>
+      <c r="H107"/>
+      <c r="I107"/>
+      <c r="J107"/>
+      <c r="K107"/>
+      <c r="L107"/>
+      <c r="M107"/>
+      <c r="N107"/>
+    </row>
+    <row r="109" spans="1:14">
+      <c r="A109" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="107" spans="1:14">
-      <c r="A107" s="2" t="s">
+    <row r="110" spans="1:14">
+      <c r="A110" s="2" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="L61:L62"/>
-    <mergeCell ref="M61:M62"/>
+    <mergeCell ref="L64:L65"/>
+    <mergeCell ref="M64:M65"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.45" right="0.45" top="0.25" bottom="0.25" header="0.05" footer="0.05"/>
@@ -5692,7 +5833,7 @@
     <oddFooter>&amp;R&amp;8&amp;F</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="55" max="16383" man="1"/>
+    <brk id="58" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
changed the device IDs
</commit_message>
<xml_diff>
--- a/documentations/2022 coordination sheet.xlsx
+++ b/documentations/2022 coordination sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minni\Documents\GitHub\2022_prod_robot\documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C313485-79E1-4B21-A55A-193B99B45E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BF8B41-707B-4E11-85DE-0A4F1B5EFF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -995,10 +995,10 @@
     <t>PDP 15</t>
   </si>
   <si>
-    <t>PDP 14</t>
-  </si>
-  <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>PDP 13</t>
   </si>
 </sst>
 </file>
@@ -2000,23 +2000,23 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3609,7 +3609,7 @@
   <dimension ref="A1:O110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="69" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -4080,11 +4080,11 @@
       </c>
       <c r="G15" s="32"/>
       <c r="H15" s="32" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>169</v>
@@ -4111,11 +4111,11 @@
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K16" s="12" t="s">
         <v>169</v>
@@ -4146,7 +4146,7 @@
       </c>
       <c r="I17" s="32"/>
       <c r="J17" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K17" s="12" t="s">
         <v>169</v>
@@ -4192,33 +4192,33 @@
       <c r="M18" s="33"/>
     </row>
     <row r="19" spans="1:13" s="111" customFormat="1">
-      <c r="A19" s="114" t="s">
+      <c r="A19" s="112" t="s">
         <v>194</v>
       </c>
-      <c r="B19" s="115" t="s">
+      <c r="B19" s="113" t="s">
         <v>195</v>
       </c>
       <c r="C19" s="107" t="s">
         <v>196</v>
       </c>
       <c r="D19" s="108"/>
-      <c r="E19" s="115"/>
+      <c r="E19" s="113"/>
       <c r="F19" s="109" t="s">
         <v>197</v>
       </c>
-      <c r="G19" s="115" t="s">
+      <c r="G19" s="113" t="s">
         <v>198</v>
       </c>
-      <c r="H19" s="115" t="s">
+      <c r="H19" s="113" t="s">
         <v>196</v>
       </c>
-      <c r="I19" s="116"/>
-      <c r="J19" s="115" t="s">
+      <c r="I19" s="114"/>
+      <c r="J19" s="113" t="s">
         <v>120</v>
       </c>
       <c r="K19" s="106"/>
       <c r="L19" s="109"/>
-      <c r="M19" s="117"/>
+      <c r="M19" s="115"/>
     </row>
     <row r="20" spans="1:13" ht="24.6" thickBot="1">
       <c r="A20" s="5" t="s">
@@ -5057,10 +5057,10 @@
       <c r="I64" s="45"/>
       <c r="J64" s="45"/>
       <c r="K64" s="60"/>
-      <c r="L64" s="112" t="s">
+      <c r="L64" s="116" t="s">
         <v>75</v>
       </c>
-      <c r="M64" s="113" t="s">
+      <c r="M64" s="117" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5084,8 +5084,8 @@
       <c r="I65" s="39"/>
       <c r="J65" s="39"/>
       <c r="K65" s="61"/>
-      <c r="L65" s="112"/>
-      <c r="M65" s="113"/>
+      <c r="L65" s="116"/>
+      <c r="M65" s="117"/>
     </row>
     <row r="66" spans="1:15">
       <c r="A66" s="41" t="s">

</xml_diff>